<commit_message>
nuevos cambios desde oficina
</commit_message>
<xml_diff>
--- a/Desglose.xlsx
+++ b/Desglose.xlsx
@@ -359,15 +359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:D18"/>
+      <selection activeCell="C9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,6 +452,21 @@
         <v>20616.36</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2038.91</v>
+      </c>
+      <c r="C9">
+        <v>7865.64</v>
+      </c>
+      <c r="E9">
+        <v>7865.64</v>
+      </c>
+      <c r="G9">
+        <f>SUM(A9:F9)</f>
+        <v>17770.190000000002</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
desglosse del 15 al 29 de feb
</commit_message>
<xml_diff>
--- a/Desglose.xlsx
+++ b/Desglose.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Desglose de ingresos 15-31 Ener" sheetId="1" r:id="rId1"/>
     <sheet name="Desglose de ingresos 01-15 Feb" sheetId="2" r:id="rId2"/>
+    <sheet name="Desglose de ingresos 15-29 Feb" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>sueldo</t>
   </si>
@@ -375,8 +376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -685,4 +686,162 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>149.47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2145</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1202.69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1202.69</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>71.150000000000006</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>53.99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>53.99</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>SUM(A2:A6)</f>
+        <v>2473.5999999999995</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <f>SUM(C2:C6)</f>
+        <v>9048.75</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <f>SUM(E2:E6)</f>
+        <v>9048.75</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <f>SUM(A7:F7)</f>
+        <v>20571.099999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2116.0100000000002</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <f>SUM(A9:F9)</f>
+        <v>17808.13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
desglose del 01-15 abril
</commit_message>
<xml_diff>
--- a/Desglose.xlsx
+++ b/Desglose.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Desglose de ingresos 15-31 Ener" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Desglose de ingresos 15-29 Feb" sheetId="3" r:id="rId3"/>
     <sheet name="Desglose de ingresos 01-15 Mar" sheetId="4" r:id="rId4"/>
     <sheet name="Desglose de ingresos 16-31 Mar" sheetId="5" r:id="rId5"/>
+    <sheet name="Desglose de ingresos 01-15 Abr" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
   <si>
     <t>sueldo</t>
   </si>
@@ -49,6 +50,12 @@
   </si>
   <si>
     <t>tengo actual</t>
+  </si>
+  <si>
+    <t>dep1</t>
+  </si>
+  <si>
+    <t>dep2</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1019,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1176,4 +1183,62 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2157.37</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>7826.98</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>7826.98</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <f>SUM(A2:F2)</f>
+        <v>17811.329999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
desglose del 16-30 de abril
</commit_message>
<xml_diff>
--- a/Desglose.xlsx
+++ b/Desglose.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Desglose de ingresos 15-31 Ener" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Desglose de ingresos 01-15 Mar" sheetId="4" r:id="rId4"/>
     <sheet name="Desglose de ingresos 16-31 Mar" sheetId="5" r:id="rId5"/>
     <sheet name="Desglose de ingresos 01-15 Abr" sheetId="6" r:id="rId6"/>
+    <sheet name="Desglose de ingresos 16-30 Abri" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="9">
   <si>
     <t>sueldo</t>
   </si>
@@ -1189,7 +1190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1241,4 +1242,165 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>149.47</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2145</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1202.69</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1202.69</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>71.150000000000006</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>53.99</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>53.25</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f>SUM(A2:A6)</f>
+        <v>2472.8599999999997</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
+        <f>SUM(C2:C6)</f>
+        <v>9048.75</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <f>SUM(E2:E6)</f>
+        <v>9048.75</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <f>SUM(A7:F7)</f>
+        <v>20570.36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2108.91</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>7846.06</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <f>SUM(A9:F9)</f>
+        <v>17801.030000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>